<commit_message>
Refactor to new data structure
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Lokal/Flutter/rag_tco/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678FB113-AE8E-E040-9289-0258EBC8D850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C524C-43D9-B441-97CC-92E7257BF9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19780" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
+    <workbookView xWindow="36580" yWindow="500" windowWidth="34560" windowHeight="19300" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
   </bookViews>
   <sheets>
-    <sheet name="provider" sheetId="1" r:id="rId1"/>
+    <sheet name="languageModel" sheetId="1" r:id="rId1"/>
     <sheet name="serviceTemplates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="28">
   <si>
     <t>GPT-4o</t>
   </si>
@@ -75,21 +75,12 @@
     <t>Picture</t>
   </si>
   <si>
-    <t>Video Input</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
     <t>Text Input</t>
   </si>
   <si>
     <t>Characters</t>
   </si>
   <si>
-    <t>Audio Input</t>
-  </si>
-  <si>
     <t>Gemini 1.5 Pro (=&lt; 128.000 Context Window)</t>
   </si>
   <si>
@@ -112,6 +103,24 @@
   </si>
   <si>
     <t>Large Report</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -493,14 +502,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF7FF2C-6B96-8844-9EA7-07D3B31EAAF5}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="2" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -508,28 +517,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1">
         <v>5</v>
       </c>
-      <c r="D1">
-        <v>1000000</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
+      <c r="E1">
+        <v>1000000</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1">
         <v>15</v>
       </c>
-      <c r="H1">
-        <v>1000000</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
+      <c r="I1">
+        <v>1000000</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -537,28 +546,28 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
         <v>2.5</v>
       </c>
-      <c r="D2">
-        <v>1000000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
+      <c r="E2">
+        <v>1000000</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>1000000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
+      <c r="I2">
+        <v>1000000</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -566,28 +575,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
         <v>0.15</v>
       </c>
-      <c r="D3">
-        <v>1000000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
+      <c r="E3">
+        <v>1000000</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
         <v>0.6</v>
       </c>
-      <c r="H3">
-        <v>1000000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
+      <c r="I3">
+        <v>1000000</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -595,28 +604,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
         <v>0.08</v>
       </c>
-      <c r="D4">
-        <v>1000000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
+      <c r="E4">
+        <v>1000000</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
         <v>0.3</v>
       </c>
-      <c r="H4">
-        <v>1000000</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
+      <c r="I4">
+        <v>1000000</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -624,28 +633,28 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
         <v>0.5</v>
       </c>
-      <c r="D5">
-        <v>1000000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
+      <c r="E5">
+        <v>1000000</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
         <v>1.5</v>
       </c>
-      <c r="H5">
-        <v>1000000</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
+      <c r="I5">
+        <v>1000000</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -653,28 +662,28 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
         <v>0.25</v>
       </c>
-      <c r="D6">
-        <v>1000000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
+      <c r="E6">
+        <v>1000000</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6">
         <v>0.75</v>
       </c>
-      <c r="H6">
-        <v>1000000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1</v>
+      <c r="I6">
+        <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -682,28 +691,28 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
         <v>1.5</v>
       </c>
-      <c r="D7">
-        <v>1000000</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
+      <c r="E7">
+        <v>1000000</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
-        <v>1000000</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
+      <c r="I7">
+        <v>1000000</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -711,341 +720,341 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
         <v>0.75</v>
       </c>
-      <c r="D8">
-        <v>1000000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
+      <c r="E8">
+        <v>1000000</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
       </c>
       <c r="H8">
-        <v>1000000</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1000000</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>1.315E-4</v>
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
+        <v>1.315E-3</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>1.315E-4</v>
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
+        <v>1.315E-3</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9">
+        <v>1.25E-3</v>
+      </c>
+      <c r="M9">
+        <v>250</v>
+      </c>
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9">
         <v>1.25E-4</v>
       </c>
-      <c r="L9">
-        <v>1000</v>
-      </c>
-      <c r="M9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9">
-        <v>1.2500000000000001E-5</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>13</v>
+      <c r="Q9">
+        <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>21</v>
-      </c>
-      <c r="S9">
-        <v>3.7500000000000001E-4</v>
+        <v>24</v>
+      </c>
+      <c r="S9" t="s">
+        <v>23</v>
       </c>
       <c r="T9">
-        <v>1000</v>
-      </c>
-      <c r="U9" t="s">
-        <v>15</v>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="U9">
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.63E-4</v>
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2.63E-4</v>
+        <v>2.63E-3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
       </c>
       <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="1">
+        <v>2.63E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="M10">
+        <v>250</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="1">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="L10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="1">
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="P10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>13</v>
+      <c r="Q10" s="1">
+        <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>21</v>
-      </c>
-      <c r="S10">
-        <v>7.5000000000000002E-4</v>
+        <v>24</v>
+      </c>
+      <c r="S10" t="s">
+        <v>23</v>
       </c>
       <c r="T10">
-        <v>1000</v>
-      </c>
-      <c r="U10" t="s">
-        <v>15</v>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="U10">
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1.315E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1.315E-3</v>
+        <v>1.315E-4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
       </c>
       <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1.25E-3</v>
+        <v>1.315E-4</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
       </c>
       <c r="L11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="1">
         <v>1.25E-4</v>
       </c>
+      <c r="M11">
+        <v>250</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" t="s">
+        <v>26</v>
+      </c>
       <c r="P11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>13</v>
+        <v>1.2500000000000001E-5</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>21</v>
-      </c>
-      <c r="S11">
-        <v>3.7499999999999999E-3</v>
+        <v>24</v>
+      </c>
+      <c r="S11" t="s">
+        <v>23</v>
       </c>
       <c r="T11">
-        <v>1000</v>
-      </c>
-      <c r="U11" t="s">
-        <v>15</v>
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="U11">
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.63E-3</v>
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2.63E-3</v>
+        <v>2.63E-4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
       </c>
       <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="1">
-        <v>2.5000000000000001E-3</v>
+        <v>2.63E-4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
       </c>
       <c r="L12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="1">
         <v>2.5000000000000001E-4</v>
       </c>
+      <c r="M12">
+        <v>250</v>
+      </c>
+      <c r="N12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" t="s">
+        <v>26</v>
+      </c>
       <c r="P12" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>13</v>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>21</v>
-      </c>
-      <c r="S12">
-        <v>7.4999999999999997E-3</v>
+        <v>24</v>
+      </c>
+      <c r="S12" t="s">
+        <v>23</v>
       </c>
       <c r="T12">
-        <v>1000</v>
-      </c>
-      <c r="U12" t="s">
-        <v>15</v>
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="U12">
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1">
         <v>2E-3</v>
       </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1">
         <v>1.25E-4</v>
       </c>
-      <c r="L13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>15</v>
+      <c r="M13">
+        <v>250</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="1">
+        <v>24</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="1">
         <v>3.7500000000000001E-4</v>
       </c>
-      <c r="P13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>15</v>
+      <c r="Q13" s="1">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1055,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D9F702-5D64-F841-8192-06624ACC7561}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,12 +1075,12 @@
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1">
         <v>50000</v>
@@ -1080,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1">
         <v>200000</v>
@@ -1088,13 +1097,31 @@
       <c r="G1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>100000</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1">
+        <v>200000</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>300000</v>
@@ -1103,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>500000</v>
@@ -1111,10 +1138,28 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>300000</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <v>600000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1126,13 +1171,13 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>2000</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Fix Cost Elements
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Lokal/Flutter/rag_tco/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C524C-43D9-B441-97CC-92E7257BF9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9497E3F9-FC40-3F4D-8E58-94809BB28781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36580" yWindow="500" windowWidth="34560" windowHeight="19300" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="19300" activeTab="5" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
   </bookViews>
   <sheets>
     <sheet name="languageModel" sheetId="1" r:id="rId1"/>
-    <sheet name="serviceTemplates" sheetId="2" r:id="rId2"/>
+    <sheet name="retriever" sheetId="4" r:id="rId2"/>
+    <sheet name="reranker" sheetId="3" r:id="rId3"/>
+    <sheet name="storage" sheetId="5" r:id="rId4"/>
+    <sheet name="vectorDB" sheetId="6" r:id="rId5"/>
+    <sheet name="preprocessor" sheetId="7" r:id="rId6"/>
+    <sheet name="serviceTemplates" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="49">
   <si>
     <t>GPT-4o</t>
   </si>
@@ -121,13 +126,76 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Compression .25</t>
+  </si>
+  <si>
+    <t>Compression .75</t>
+  </si>
+  <si>
+    <t>Compression .50</t>
+  </si>
+  <si>
+    <t>Compression</t>
+  </si>
+  <si>
+    <t>Fix Doc 50</t>
+  </si>
+  <si>
+    <t>FixDoc</t>
+  </si>
+  <si>
+    <t>Fix Doc 100</t>
+  </si>
+  <si>
+    <t>Fix Doc 200</t>
+  </si>
+  <si>
+    <t>Compression 1</t>
+  </si>
+  <si>
+    <t>50x1000</t>
+  </si>
+  <si>
+    <t>100x2000</t>
+  </si>
+  <si>
+    <t>200x3000</t>
+  </si>
+  <si>
+    <t>Storage 1</t>
+  </si>
+  <si>
+    <t>Storage 0.25</t>
+  </si>
+  <si>
+    <t>Storage 5</t>
+  </si>
+  <si>
+    <t>VectorDB 0.25</t>
+  </si>
+  <si>
+    <t>VectorDB 1</t>
+  </si>
+  <si>
+    <t>VectorDB 5</t>
+  </si>
+  <si>
+    <t>Preprocessor 0.25</t>
+  </si>
+  <si>
+    <t>Preprocessor 1</t>
+  </si>
+  <si>
+    <t>Preprocessor 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +206,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF7FF2C-6B96-8844-9EA7-07D3B31EAAF5}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="159" workbookViewId="0">
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
@@ -1063,6 +1137,274 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542711A6-8D29-2945-A02A-0019C3303C41}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+      <c r="C1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34452647-C66C-3547-8812-D6DE19E7A6C6}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771827B2-4F6D-5541-8F76-6BD413AE1161}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23501164-5B78-CD47-A3E8-84848A0B1746}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83FA0F6-ACCA-0D41-B4EE-74416524A46E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D9F702-5D64-F841-8192-06624ACC7561}">
   <dimension ref="A1:M3"/>
   <sheetViews>

</xml_diff>